<commit_message>
Cleaned out zero terms due to differences between vert and nlppipe tagger
</commit_message>
<xml_diff>
--- a/xlsx/sauszemes_transporta_termini.xlsx
+++ b/xlsx/sauszemes_transporta_termini.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="320">
   <si>
     <t>ngram</t>
   </si>
@@ -73,9 +73,6 @@
     <t>autotaksis</t>
   </si>
   <si>
-    <t>autovāģis</t>
-  </si>
-  <si>
     <t>ātrs palīdzība auto</t>
   </si>
   <si>
@@ -181,7 +178,7 @@
     <t>dzelzsasnieks</t>
   </si>
   <si>
-    <t>dzelzsceļš rats</t>
+    <t>dzelzceļš rats</t>
   </si>
   <si>
     <t>eizenbānis</t>
@@ -211,9 +208,6 @@
     <t>elektrotraktors</t>
   </si>
   <si>
-    <t>essex roadster</t>
-  </si>
-  <si>
     <t>faetons</t>
   </si>
   <si>
@@ -229,13 +223,13 @@
     <t>fūrmanis</t>
   </si>
   <si>
-    <t>fūrmaņs kamanas</t>
-  </si>
-  <si>
-    <t>goda-rati</t>
-  </si>
-  <si>
-    <t>HarleysDavidsons</t>
+    <t>fuhrmans kamanas</t>
+  </si>
+  <si>
+    <t>gods rats</t>
+  </si>
+  <si>
+    <t>harleys</t>
   </si>
   <si>
     <t>iela autobuss</t>
@@ -319,7 +313,7 @@
     <t>motocikls ar blakusvāģis</t>
   </si>
   <si>
-    <t>motorrats</t>
+    <t>motorats</t>
   </si>
   <si>
     <t>oldsmobili</t>
@@ -373,9 +367,6 @@
     <t>ragavas</t>
   </si>
   <si>
-    <t>redelains ore</t>
-  </si>
-  <si>
     <t>redele rats</t>
   </si>
   <si>
@@ -385,16 +376,19 @@
     <t>rikšotājs</t>
   </si>
   <si>
+    <t>roadsteris</t>
+  </si>
+  <si>
     <t>rodsters</t>
   </si>
   <si>
-    <t>Roll-Rois</t>
+    <t>rol-rois</t>
   </si>
   <si>
     <t>rumaks</t>
   </si>
   <si>
-    <t>sanitars automobilis</t>
+    <t>sanitārs automobilis</t>
   </si>
   <si>
     <t>sanitartransports</t>
@@ -556,9 +550,6 @@
     <t>('autotaksis',)</t>
   </si>
   <si>
-    <t>('autovāģis',)</t>
-  </si>
-  <si>
     <t>('ātrs', 'palīdzība', 'auto')</t>
   </si>
   <si>
@@ -664,7 +655,7 @@
     <t>('dzelzsasnieks',)</t>
   </si>
   <si>
-    <t>('dzelzsceļš', 'rats')</t>
+    <t>('dzelzceļš', 'rats')</t>
   </si>
   <si>
     <t>('eizenbānis',)</t>
@@ -694,9 +685,6 @@
     <t>('elektrotraktors',)</t>
   </si>
   <si>
-    <t>('essex', 'roadster')</t>
-  </si>
-  <si>
     <t>('faetons',)</t>
   </si>
   <si>
@@ -712,13 +700,13 @@
     <t>('fūrmanis',)</t>
   </si>
   <si>
-    <t>('fūrmaņs', 'kamanas')</t>
-  </si>
-  <si>
-    <t>('goda-rati',)</t>
-  </si>
-  <si>
-    <t>('HarleysDavidsons',)</t>
+    <t>('fuhrmans', 'kamanas')</t>
+  </si>
+  <si>
+    <t>('gods', 'rats')</t>
+  </si>
+  <si>
+    <t>('harleys',)</t>
   </si>
   <si>
     <t>('iela', 'autobuss')</t>
@@ -802,7 +790,7 @@
     <t>('motocikls', 'ar', 'blakusvāģis')</t>
   </si>
   <si>
-    <t>('motorrats',)</t>
+    <t>('motorats',)</t>
   </si>
   <si>
     <t>('oldsmobili',)</t>
@@ -856,9 +844,6 @@
     <t>('ragavas',)</t>
   </si>
   <si>
-    <t>('redelains', 'ore')</t>
-  </si>
-  <si>
     <t>('redele', 'rats')</t>
   </si>
   <si>
@@ -868,16 +853,19 @@
     <t>('rikšotājs',)</t>
   </si>
   <si>
+    <t>('roadsteris',)</t>
+  </si>
+  <si>
     <t>('rodsters',)</t>
   </si>
   <si>
-    <t>('Roll-Rois',)</t>
+    <t>('rol-rois',)</t>
   </si>
   <si>
     <t>('rumaks',)</t>
   </si>
   <si>
-    <t>('sanitars', 'automobilis')</t>
+    <t>('sanitārs', 'automobilis')</t>
   </si>
   <si>
     <t>('sanitartransports',)</t>
@@ -1343,7 +1331,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:D159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1368,10 +1356,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
         <v>163</v>
-      </c>
-      <c r="C2" t="s">
-        <v>165</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -1382,10 +1370,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
         <v>164</v>
-      </c>
-      <c r="C3" t="s">
-        <v>166</v>
       </c>
       <c r="D3">
         <v>13</v>
@@ -1396,10 +1384,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4">
         <v>5557</v>
@@ -1410,10 +1398,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1424,10 +1412,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D6">
         <v>230</v>
@@ -1438,10 +1426,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D7">
         <v>9</v>
@@ -1452,10 +1440,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1466,10 +1454,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1480,10 +1468,10 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D10">
         <v>38</v>
@@ -1494,10 +1482,10 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11">
         <v>1316</v>
@@ -1508,10 +1496,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D12">
         <v>69</v>
@@ -1522,10 +1510,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -1536,10 +1524,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D14">
         <v>59</v>
@@ -1550,10 +1538,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1564,10 +1552,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D16">
         <v>11</v>
@@ -1578,13 +1566,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1592,13 +1580,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1606,13 +1594,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1620,13 +1608,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1634,13 +1622,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1648,13 +1636,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D22">
-        <v>85</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1662,13 +1650,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1676,13 +1664,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>437</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1690,13 +1678,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D25">
-        <v>437</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1704,13 +1692,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1718,13 +1706,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D27">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1732,13 +1720,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D28">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1746,13 +1734,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D29">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1760,13 +1748,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D30">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1774,13 +1762,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1788,13 +1776,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D32">
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1802,10 +1790,10 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -1816,13 +1804,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1830,13 +1818,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D35">
-        <v>14</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1844,13 +1832,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C36" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D36">
-        <v>238</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1858,13 +1846,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1872,13 +1860,13 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D38">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1886,13 +1874,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1900,13 +1888,13 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C40" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1914,13 +1902,13 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D41">
-        <v>63</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1928,13 +1916,13 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C42" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D42">
-        <v>160</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1942,13 +1930,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1956,13 +1944,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1970,13 +1958,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C45" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1984,13 +1972,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D46">
-        <v>4</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1998,13 +1986,13 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C47" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D47">
-        <v>248</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2012,13 +2000,13 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D48">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2026,13 +2014,13 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D49">
-        <v>19</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2040,13 +2028,13 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D50">
-        <v>1116</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2054,13 +2042,13 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C51" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D51">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2068,13 +2056,13 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C52" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2082,13 +2070,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C53" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2096,13 +2084,13 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D54">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2110,13 +2098,13 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C55" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2124,13 +2112,13 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D56">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2138,10 +2126,10 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C57" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2152,10 +2140,10 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C58" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2166,13 +2154,13 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C59" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2180,13 +2168,13 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C60" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D60">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2194,13 +2182,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C61" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D61">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2208,13 +2196,13 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2222,13 +2210,13 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C63" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2236,13 +2224,13 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D64">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2250,10 +2238,10 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C65" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D65">
         <v>4</v>
@@ -2264,13 +2252,13 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C66" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D66">
-        <v>93</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2278,13 +2266,13 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C67" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2292,13 +2280,13 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C68" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D68">
-        <v>138</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2306,13 +2294,13 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C69" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2320,13 +2308,13 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C70" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2334,13 +2322,13 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C71" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2348,13 +2336,13 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C72" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2362,13 +2350,13 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C73" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D73">
-        <v>21</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2376,13 +2364,13 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C74" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D74">
-        <v>93</v>
+        <v>638</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2390,13 +2378,13 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C75" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D75">
-        <v>1116</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2404,13 +2392,13 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C76" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D76">
-        <v>638</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2418,13 +2406,13 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C77" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D77">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2432,13 +2420,13 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C78" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D78">
-        <v>22</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2446,13 +2434,13 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C79" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D79">
-        <v>23</v>
+        <v>939</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2460,13 +2448,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C80" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D80">
-        <v>203</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2474,13 +2462,13 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C81" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D81">
-        <v>939</v>
+        <v>396</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2488,13 +2476,13 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C82" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D82">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2502,13 +2490,13 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C83" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D83">
-        <v>396</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2516,13 +2504,13 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C84" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D84">
-        <v>67</v>
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2530,13 +2518,13 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C85" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D85">
-        <v>80</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2544,13 +2532,13 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C86" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D86">
-        <v>122</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2558,41 +2546,41 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C87" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D87">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C88" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D88">
-        <v>53</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C89" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D89">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2600,13 +2588,13 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C90" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D90">
-        <v>12</v>
+        <v>247</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2614,13 +2602,13 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C91" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D91">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2628,13 +2616,13 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C92" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D92">
-        <v>247</v>
+        <v>303</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2642,13 +2630,13 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C93" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D93">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2656,13 +2644,13 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
+        <v>161</v>
+      </c>
+      <c r="C94" t="s">
+        <v>254</v>
+      </c>
+      <c r="D94">
         <v>164</v>
-      </c>
-      <c r="C94" t="s">
-        <v>256</v>
-      </c>
-      <c r="D94">
-        <v>303</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2670,13 +2658,13 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C95" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2684,13 +2672,13 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C96" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D96">
-        <v>164</v>
+        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2698,13 +2686,13 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C97" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D97">
-        <v>74</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2712,13 +2700,13 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C98" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D98">
-        <v>86</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2726,10 +2714,10 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C99" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -2740,13 +2728,13 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C100" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2754,13 +2742,13 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C101" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>19872</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2768,13 +2756,13 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C102" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D102">
-        <v>10</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2782,13 +2770,13 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C103" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D103">
-        <v>19872</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2796,13 +2784,13 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C104" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D104">
-        <v>1070</v>
+        <v>43</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2810,13 +2798,13 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C105" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2824,13 +2812,13 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C106" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D106">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2838,13 +2826,13 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C107" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D107">
-        <v>15</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2852,13 +2840,13 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C108" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D108">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2866,13 +2854,13 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C109" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D109">
-        <v>1485</v>
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2880,13 +2868,13 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C110" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D110">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2894,13 +2882,13 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C111" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D111">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2908,13 +2896,13 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C112" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2922,13 +2910,13 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C113" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D113">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2936,13 +2924,13 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C114" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D114">
-        <v>2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2950,13 +2938,13 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C115" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D115">
-        <v>37</v>
+        <v>821</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2964,13 +2952,13 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C116" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D116">
-        <v>72</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2978,13 +2966,13 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C117" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D117">
-        <v>821</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2992,13 +2980,13 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C118" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3006,13 +2994,13 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C119" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D119">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3020,13 +3008,13 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C120" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D120">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3034,13 +3022,13 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C121" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D121">
-        <v>63</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3048,13 +3036,13 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C122" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D122">
-        <v>2</v>
+        <v>217</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3062,13 +3050,13 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C123" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3076,13 +3064,13 @@
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C124" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D124">
-        <v>217</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3090,13 +3078,13 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C125" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3104,13 +3092,13 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C126" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3118,13 +3106,13 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C127" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3132,13 +3120,13 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C128" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D128">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3146,13 +3134,13 @@
         <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C129" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D129">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3160,10 +3148,10 @@
         <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C130" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -3174,13 +3162,13 @@
         <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C131" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D131">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3188,13 +3176,13 @@
         <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C132" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>149</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3202,13 +3190,13 @@
         <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C133" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3216,13 +3204,13 @@
         <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C134" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D134">
-        <v>149</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3230,13 +3218,13 @@
         <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C135" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D135">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3244,13 +3232,13 @@
         <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C136" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D136">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3258,13 +3246,13 @@
         <v>138</v>
       </c>
       <c r="B137" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C137" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D137">
-        <v>95</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3272,13 +3260,13 @@
         <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C138" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D138">
-        <v>18</v>
+        <v>223</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3286,13 +3274,13 @@
         <v>140</v>
       </c>
       <c r="B139" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C139" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D139">
-        <v>12</v>
+        <v>151</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3300,13 +3288,13 @@
         <v>141</v>
       </c>
       <c r="B140" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C140" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D140">
-        <v>223</v>
+        <v>110</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3314,13 +3302,13 @@
         <v>142</v>
       </c>
       <c r="B141" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C141" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D141">
-        <v>151</v>
+        <v>579</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3328,13 +3316,13 @@
         <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C142" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D142">
-        <v>110</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3342,13 +3330,13 @@
         <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C143" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D143">
-        <v>579</v>
+        <v>315</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3356,13 +3344,13 @@
         <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C144" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D144">
-        <v>3</v>
+        <v>62</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3370,13 +3358,13 @@
         <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C145" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D145">
-        <v>315</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3384,13 +3372,13 @@
         <v>147</v>
       </c>
       <c r="B146" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C146" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D146">
-        <v>62</v>
+        <v>394</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3398,13 +3386,13 @@
         <v>148</v>
       </c>
       <c r="B147" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C147" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D147">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3412,13 +3400,13 @@
         <v>149</v>
       </c>
       <c r="B148" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C148" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D148">
-        <v>394</v>
+        <v>54</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3426,13 +3414,13 @@
         <v>150</v>
       </c>
       <c r="B149" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C149" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D149">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3440,13 +3428,13 @@
         <v>151</v>
       </c>
       <c r="B150" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C150" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D150">
-        <v>54</v>
+        <v>443</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3454,13 +3442,13 @@
         <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C151" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D151">
-        <v>56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3468,13 +3456,13 @@
         <v>153</v>
       </c>
       <c r="B152" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C152" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D152">
-        <v>443</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3482,13 +3470,13 @@
         <v>154</v>
       </c>
       <c r="B153" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C153" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3496,13 +3484,13 @@
         <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C154" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D154">
-        <v>3187</v>
+        <v>4868</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3510,13 +3498,13 @@
         <v>156</v>
       </c>
       <c r="B155" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C155" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D155">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3524,13 +3512,13 @@
         <v>157</v>
       </c>
       <c r="B156" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C156" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D156">
-        <v>4868</v>
+        <v>577</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3538,13 +3526,13 @@
         <v>158</v>
       </c>
       <c r="B157" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C157" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D157">
-        <v>6</v>
+        <v>19102</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3552,13 +3540,13 @@
         <v>159</v>
       </c>
       <c r="B158" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C158" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D158">
-        <v>577</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3566,40 +3554,12 @@
         <v>160</v>
       </c>
       <c r="B159" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C159" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D159">
-        <v>19102</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="A160" t="s">
-        <v>161</v>
-      </c>
-      <c r="B160" t="s">
-        <v>164</v>
-      </c>
-      <c r="C160" t="s">
-        <v>322</v>
-      </c>
-      <c r="D160">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
-      <c r="A161" t="s">
-        <v>162</v>
-      </c>
-      <c r="B161" t="s">
-        <v>164</v>
-      </c>
-      <c r="C161" t="s">
-        <v>323</v>
-      </c>
-      <c r="D161">
         <v>142</v>
       </c>
     </row>

</xml_diff>